<commit_message>
Megan before class July 28
</commit_message>
<xml_diff>
--- a/Project 1 Analysis and To Do List.xlsx
+++ b/Project 1 Analysis and To Do List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Documents\DataBootCamp_Projects\Group_5_Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D53F95-CD25-41E7-8BB6-35AC307A25F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF636237-4E8E-430C-9DCE-8FCF363939F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88D9DF25-7171-4E3D-82B5-93F9BDD9EFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{88D9DF25-7171-4E3D-82B5-93F9BDD9EFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="To Do List" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Project Task</t>
   </si>
@@ -163,14 +163,78 @@
   </si>
   <si>
     <t>make sure 1933 best picture film included</t>
+  </si>
+  <si>
+    <r>
+      <t>Just under half of both the Best Picture (45%) and Top Grossing films (42%) over the past century passed the Bechdel Test.  Has this changed over time?  Maybe?  Since the turn of the century twenty years ago, of the top grossing films for each year - 14 pass the Bechdel test.  And of course the Best Picture Award winners have kept up with this trend, right?  Well, not exactly.  Since 2000, only 10 out of the 19 Academy Award Best Picture Winners pass the Bechdel Test.  
+And at the turn of the millenium?  Both the top grossing film (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mission Impossible II</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) and the Best Picture award winner (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gladiator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) FAIL the Bechdel test with a ZERO.  Which means, not only is there no conversation between 2 women in the film about something besides a man.  The films don't have more than one female character (extras don't count).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -204,12 +268,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB55FD5-ED4C-4D83-9152-AF8F7D70B817}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +623,7 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -569,7 +634,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -682,13 +747,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF779DC8-AC57-4208-AA10-495A9F41E30A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="34" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.21875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -712,9 +778,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -736,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -747,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Megan push July 29
</commit_message>
<xml_diff>
--- a/Project 1 Analysis and To Do List.xlsx
+++ b/Project 1 Analysis and To Do List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Documents\DataBootCamp_Projects\Group_5_Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D537BCF-EEAC-454E-8390-792CB04DC03F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4E11E1-6272-4EDE-A3E0-22A03D510E07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88D9DF25-7171-4E3D-82B5-93F9BDD9EFC3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{88D9DF25-7171-4E3D-82B5-93F9BDD9EFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="To Do List" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Project Task</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Number of Visualizations</t>
-  </si>
-  <si>
-    <t>Across the Internet Movie Data Base (IMDB), the ratings for top grossing films and best picture award winners are markedly similarly across the years with both pictures typically rating favorably.  Meanwhile, the Rotten Tomato "Tomatometer" shows a  greater variation between top grossing film scores and best picture film scores.  Particularly of interest are the films from ????????  Overall, best picture films score consistently favorably on the Tomatometer, whilst the more volatile score swings belong to the top grossing films.</t>
   </si>
   <si>
     <t>Megan To Do List</t>
@@ -223,6 +220,24 @@
   </si>
   <si>
     <t>Work on Presentation Slides</t>
+  </si>
+  <si>
+    <t>Across the Internet Movie Data Base (IMDB), the ratings for top grossing films and best picture award winners are markedly similarly across the years with both pictures typically rating favorably.  Meanwhile, the Rotten Tomato "Tomatometer" shows a  greater variation between top grossing film scores and best picture film scores.  Particularly of interest are the films from 2014 (Transformers 2) vs. (Birdman).  Overall, best picture films score consistently favorably on the Tomatometer, whilst the more volatile score swings belong to the top grossing films.</t>
+  </si>
+  <si>
+    <t>Bechdel Test - what is it</t>
+  </si>
+  <si>
+    <t>Bechdel pie charts</t>
+  </si>
+  <si>
+    <t>bechdel horizontal bar</t>
+  </si>
+  <si>
+    <t>Summarize Findings</t>
+  </si>
+  <si>
+    <t>General Conclusions in Slideshow</t>
   </si>
 </sst>
 </file>
@@ -280,13 +295,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB55FD5-ED4C-4D83-9152-AF8F7D70B817}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,10 +642,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -640,10 +656,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -654,10 +670,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -668,29 +684,32 @@
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>33</v>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>34</v>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -700,16 +719,22 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>35</v>
+      <c r="E7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
-        <v>36</v>
+      <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -717,13 +742,19 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -731,7 +762,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -742,27 +773,27 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -775,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF779DC8-AC57-4208-AA10-495A9F41E30A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,7 +842,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -844,12 +875,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>

</xml_diff>